<commit_message>
Cambiado columnas coste y precio unitario
</commit_message>
<xml_diff>
--- a/datos/ventas_grupos_productos_costes.xlsx
+++ b/datos/ventas_grupos_productos_costes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitatdevalencia-my.sharepoint.com/personal/jorpipe_alumni_uv_es/Documents/e. Heladería/Simulaciones de Monte Carlo para Hostelería/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_F25DC773A252ABDACC10489189DE6B545ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0643766-13C4-40E5-9525-FA7A344B0246}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC10489189DE6B545ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FED79586-7560-4654-BC21-4568974B4AA9}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="3468" windowWidth="16860" windowHeight="8136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3924" yWindow="4044" windowWidth="16860" windowHeight="8136" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ventas" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>enero</t>
   </si>
@@ -72,12 +72,6 @@
     <t>grupo</t>
   </si>
   <si>
-    <t>beneficio unitario</t>
-  </si>
-  <si>
-    <t>nivel de demanda dentro del grupo</t>
-  </si>
-  <si>
     <t>coste_fijo</t>
   </si>
   <si>
@@ -88,6 +82,15 @@
   </si>
   <si>
     <t>mes</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>coste_unitario</t>
+  </si>
+  <si>
+    <t>nivel_demanda_dentro_de_grupo</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3DED08-916A-4BC6-960A-3F5966AE9FC0}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -471,10 +474,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -545,7 +548,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5"/>
     </row>
@@ -558,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +620,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -633,10 +636,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872FC0EC-CEC1-4AB6-B770-65C1FE8B5816}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,10 +647,11 @@
     <col min="1" max="1" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -655,15 +659,18 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{13970312-68AA-4EAB-8537-96ECA2DD4235}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{13970312-68AA-4EAB-8537-96ECA2DD4235}">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -710,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -746,7 +753,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadido gráficos de la parte del analisis de datos no simulados
</commit_message>
<xml_diff>
--- a/datos/ventas_grupos_productos_costes.xlsx
+++ b/datos/ventas_grupos_productos_costes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitatdevalencia-my.sharepoint.com/personal/jorpipe_alumni_uv_es/Documents/e. Heladería/Simulaciones de Monte Carlo para Hostelería/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_F25DC773A252ABDACC10489189DE6B545ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79CDF88B-0079-4371-B3C0-17C78305A6E6}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_F25DC773A252ABDACC10489189DE6B545ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE078946-6382-4C85-8A80-8334608D16E7}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1872" windowWidth="16860" windowHeight="8136" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ventas" sheetId="4" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>diciembre</t>
   </si>
   <si>
-    <t>ventas_totales</t>
-  </si>
-  <si>
     <t>mes</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>coste_indirecto</t>
+  </si>
+  <si>
+    <t>ingresos_totales</t>
   </si>
 </sst>
 </file>
@@ -462,22 +462,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3DED08-916A-4BC6-960A-3F5966AE9FC0}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,13 +659,13 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0BF44F-D4A6-4E8D-B10B-65E479E64F54}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -717,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>

</xml_diff>